<commit_message>
Inciso 2 y 3 completos
Se completó el laboratorio 1.
</commit_message>
<xml_diff>
--- a/File Importing/11-2018.xlsx
+++ b/File Importing/11-2018.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JR29\Documents\GitHub\data-wrangling\data\01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0ac03d24fdcff188/Documentos/Labs_DataWranglig/File Importing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{720B4714-721E-43F9-A8E7-D7F01125E643}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{720B4714-721E-43F9-A8E7-D7F01125E643}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2ABC7629-3E7B-4F5E-941E-8D228BEDEA87}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10110" xr2:uid="{DFAE85DC-F2DA-4B73-B8F3-DFCA4FCF1DA1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DFAE85DC-F2DA-4B73-B8F3-DFCA4FCF1DA1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -149,7 +149,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -186,14 +186,14 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle name="Moneda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -210,7 +210,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -510,9 +510,12 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="50.5546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -541,7 +544,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>10001984</v>
       </c>
@@ -567,7 +570,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>10001985</v>
       </c>
@@ -593,7 +596,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>10001986</v>
       </c>
@@ -619,7 +622,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>10001987</v>
       </c>
@@ -645,7 +648,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>10001988</v>
       </c>
@@ -671,7 +674,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>10001989</v>
       </c>
@@ -697,7 +700,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>10001990</v>
       </c>
@@ -723,7 +726,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>10001991</v>
       </c>
@@ -749,7 +752,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>10001992</v>
       </c>
@@ -775,7 +778,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10001993</v>
       </c>
@@ -801,7 +804,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10001994</v>
       </c>
@@ -827,7 +830,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>10001995</v>
       </c>
@@ -853,7 +856,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>10001996</v>
       </c>
@@ -879,7 +882,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>10001997</v>
       </c>
@@ -905,7 +908,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>10001998</v>
       </c>
@@ -931,7 +934,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>10001999</v>
       </c>
@@ -957,7 +960,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>10002000</v>
       </c>
@@ -983,7 +986,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>10002001</v>
       </c>
@@ -1009,7 +1012,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>10002002</v>
       </c>
@@ -1035,7 +1038,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>10002003</v>
       </c>
@@ -1061,7 +1064,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>10002004</v>
       </c>
@@ -1087,7 +1090,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>10002005</v>
       </c>
@@ -1113,7 +1116,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>10002006</v>
       </c>
@@ -1139,7 +1142,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>10002007</v>
       </c>
@@ -1165,7 +1168,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>10002008</v>
       </c>
@@ -1191,7 +1194,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>10002009</v>
       </c>
@@ -1217,7 +1220,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>10002010</v>
       </c>
@@ -1243,7 +1246,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>10002011</v>
       </c>
@@ -1269,7 +1272,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>10002012</v>
       </c>
@@ -1295,7 +1298,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>10002013</v>
       </c>
@@ -1321,7 +1324,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>10002014</v>
       </c>
@@ -1347,7 +1350,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>10002015</v>
       </c>
@@ -1373,7 +1376,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>10002016</v>
       </c>
@@ -1399,7 +1402,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>10002017</v>
       </c>
@@ -1425,7 +1428,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>10002018</v>
       </c>
@@ -1451,7 +1454,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>10002019</v>
       </c>
@@ -1477,7 +1480,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>10002020</v>
       </c>
@@ -1503,7 +1506,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>10002021</v>
       </c>
@@ -1529,7 +1532,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>10002022</v>
       </c>
@@ -1555,7 +1558,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>10002023</v>
       </c>
@@ -1581,7 +1584,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>10002024</v>
       </c>
@@ -1607,7 +1610,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>10002025</v>
       </c>
@@ -1633,7 +1636,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>10002026</v>
       </c>
@@ -1659,7 +1662,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>10002027</v>
       </c>
@@ -1685,7 +1688,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>10002028</v>
       </c>
@@ -1711,7 +1714,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>10002029</v>
       </c>
@@ -1737,7 +1740,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>10002030</v>
       </c>
@@ -1763,7 +1766,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>10002031</v>
       </c>
@@ -1789,7 +1792,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>10002032</v>
       </c>
@@ -1815,7 +1818,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>10002033</v>
       </c>
@@ -1841,7 +1844,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>10002034</v>
       </c>
@@ -1867,7 +1870,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>10002035</v>
       </c>
@@ -1893,7 +1896,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>10002036</v>
       </c>
@@ -1919,7 +1922,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>10002037</v>
       </c>
@@ -1945,7 +1948,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>10002038</v>
       </c>
@@ -1971,7 +1974,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>10002039</v>
       </c>
@@ -1997,7 +2000,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>10002040</v>
       </c>
@@ -2023,7 +2026,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>10002041</v>
       </c>
@@ -2049,7 +2052,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>10002042</v>
       </c>
@@ -2075,7 +2078,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>10002043</v>
       </c>
@@ -2101,7 +2104,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>10002044</v>
       </c>
@@ -2127,7 +2130,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>10002045</v>
       </c>
@@ -2153,7 +2156,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>10002046</v>
       </c>
@@ -2179,7 +2182,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>10002047</v>
       </c>
@@ -2205,7 +2208,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>10002048</v>
       </c>
@@ -2231,7 +2234,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>10002049</v>
       </c>
@@ -2257,7 +2260,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>10002050</v>
       </c>
@@ -2283,7 +2286,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>10002051</v>
       </c>
@@ -2309,7 +2312,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>10002052</v>
       </c>
@@ -2335,7 +2338,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>10002053</v>
       </c>
@@ -2361,7 +2364,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>10002054</v>
       </c>
@@ -2387,7 +2390,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>10002055</v>
       </c>
@@ -2413,7 +2416,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>10002056</v>
       </c>
@@ -2439,7 +2442,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>10002057</v>
       </c>
@@ -2465,7 +2468,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>10002058</v>
       </c>
@@ -2491,7 +2494,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>10002059</v>
       </c>
@@ -2517,7 +2520,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>10002060</v>
       </c>
@@ -2543,7 +2546,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>10002061</v>
       </c>
@@ -2569,7 +2572,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>10002062</v>
       </c>
@@ -2595,7 +2598,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>10002063</v>
       </c>
@@ -2621,7 +2624,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>10002064</v>
       </c>
@@ -2647,7 +2650,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>10002065</v>
       </c>
@@ -2673,7 +2676,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>10002066</v>
       </c>
@@ -2699,7 +2702,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>10002067</v>
       </c>
@@ -2725,7 +2728,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>10002068</v>
       </c>
@@ -2751,7 +2754,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>10002069</v>
       </c>
@@ -2777,7 +2780,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>10002070</v>
       </c>
@@ -2803,7 +2806,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>10002071</v>
       </c>
@@ -2829,7 +2832,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>10002072</v>
       </c>
@@ -2855,7 +2858,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>10002073</v>
       </c>
@@ -2881,7 +2884,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>10002074</v>
       </c>
@@ -2907,7 +2910,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>10002075</v>
       </c>
@@ -2933,7 +2936,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>10002076</v>
       </c>
@@ -2959,7 +2962,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>10002077</v>
       </c>
@@ -2985,7 +2988,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>10002078</v>
       </c>
@@ -3011,7 +3014,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>10002079</v>
       </c>
@@ -3037,7 +3040,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>10002080</v>
       </c>
@@ -3063,7 +3066,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>10002081</v>
       </c>
@@ -3089,7 +3092,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>10002082</v>
       </c>
@@ -3115,7 +3118,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>10002083</v>
       </c>
@@ -3141,7 +3144,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>10002084</v>
       </c>
@@ -3167,7 +3170,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>10002085</v>
       </c>
@@ -3193,7 +3196,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>10002086</v>
       </c>
@@ -3219,7 +3222,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>10002087</v>
       </c>
@@ -3245,7 +3248,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>10002088</v>
       </c>
@@ -3271,7 +3274,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>10002089</v>
       </c>
@@ -3297,7 +3300,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>10002090</v>
       </c>
@@ -3323,7 +3326,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>10002091</v>
       </c>
@@ -3349,7 +3352,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>10002092</v>
       </c>
@@ -3375,7 +3378,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>10002093</v>
       </c>
@@ -3401,7 +3404,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>10002094</v>
       </c>
@@ -3427,7 +3430,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>10002095</v>
       </c>
@@ -3453,7 +3456,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>10002096</v>
       </c>
@@ -3479,7 +3482,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>10002097</v>
       </c>
@@ -3505,7 +3508,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>10002098</v>
       </c>
@@ -3531,7 +3534,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>10002099</v>
       </c>
@@ -3557,7 +3560,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>10002100</v>
       </c>
@@ -3583,7 +3586,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>10002101</v>
       </c>
@@ -3609,7 +3612,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>10002102</v>
       </c>
@@ -3635,7 +3638,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>10002103</v>
       </c>
@@ -3661,7 +3664,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>10002104</v>
       </c>
@@ -3687,7 +3690,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>10002105</v>
       </c>
@@ -3713,7 +3716,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>10002106</v>
       </c>
@@ -3739,7 +3742,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>10002107</v>
       </c>
@@ -3765,7 +3768,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>10002108</v>
       </c>
@@ -3791,7 +3794,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>10002109</v>
       </c>
@@ -3817,7 +3820,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>10002110</v>
       </c>
@@ -3843,7 +3846,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>10002111</v>
       </c>
@@ -3869,7 +3872,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>10002112</v>
       </c>
@@ -3895,7 +3898,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>10002113</v>
       </c>
@@ -3921,7 +3924,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>10002114</v>
       </c>
@@ -3947,7 +3950,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>10002115</v>
       </c>
@@ -3973,7 +3976,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>10002116</v>
       </c>
@@ -3999,7 +4002,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>10002117</v>
       </c>
@@ -4025,7 +4028,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>10002118</v>
       </c>
@@ -4051,7 +4054,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>10002119</v>
       </c>
@@ -4077,7 +4080,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>10002120</v>
       </c>
@@ -4103,7 +4106,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>10002121</v>
       </c>
@@ -4129,7 +4132,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>10002122</v>
       </c>
@@ -4155,7 +4158,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>10002123</v>
       </c>
@@ -4181,7 +4184,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>10002124</v>
       </c>
@@ -4207,7 +4210,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>10002125</v>
       </c>
@@ -4233,7 +4236,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>10002126</v>
       </c>
@@ -4259,7 +4262,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>10002127</v>
       </c>
@@ -4285,7 +4288,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>10002128</v>
       </c>
@@ -4311,7 +4314,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>10002129</v>
       </c>
@@ -4337,7 +4340,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>10002130</v>
       </c>
@@ -4363,7 +4366,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>10002131</v>
       </c>
@@ -4389,7 +4392,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>10002132</v>
       </c>
@@ -4415,7 +4418,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>10002133</v>
       </c>
@@ -4441,7 +4444,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>10002134</v>
       </c>
@@ -4467,7 +4470,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>10002135</v>
       </c>
@@ -4493,7 +4496,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>10002136</v>
       </c>
@@ -4519,7 +4522,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>10002137</v>
       </c>
@@ -4545,7 +4548,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>10002138</v>
       </c>
@@ -4571,7 +4574,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>10002139</v>
       </c>
@@ -4597,7 +4600,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>10002140</v>
       </c>
@@ -4623,7 +4626,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>10002141</v>
       </c>
@@ -4649,7 +4652,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>10002142</v>
       </c>
@@ -4675,7 +4678,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>10002143</v>
       </c>
@@ -4701,7 +4704,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>10002144</v>
       </c>
@@ -4727,7 +4730,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>10002145</v>
       </c>
@@ -4753,7 +4756,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>10002146</v>
       </c>
@@ -4779,7 +4782,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>10002147</v>
       </c>
@@ -4805,7 +4808,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>10002148</v>
       </c>
@@ -4831,7 +4834,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>10002149</v>
       </c>
@@ -4857,7 +4860,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>10002150</v>
       </c>
@@ -4883,7 +4886,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>10002151</v>
       </c>
@@ -4909,7 +4912,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>10002152</v>
       </c>
@@ -4935,7 +4938,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>10002153</v>
       </c>
@@ -4961,7 +4964,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>10002154</v>
       </c>
@@ -4987,7 +4990,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>10002155</v>
       </c>
@@ -5013,7 +5016,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>10002156</v>
       </c>
@@ -5039,7 +5042,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>10002157</v>
       </c>
@@ -5065,7 +5068,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>10002158</v>
       </c>
@@ -5091,7 +5094,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>10002159</v>
       </c>
@@ -5117,7 +5120,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>10002160</v>
       </c>
@@ -5143,7 +5146,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>10002161</v>
       </c>
@@ -5169,7 +5172,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>10002162</v>
       </c>
@@ -5195,7 +5198,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>10002163</v>
       </c>
@@ -5221,7 +5224,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>10002164</v>
       </c>
@@ -5247,7 +5250,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>10002165</v>
       </c>
@@ -5273,7 +5276,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>10002166</v>
       </c>
@@ -5299,7 +5302,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>10002167</v>
       </c>
@@ -5325,7 +5328,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>10002168</v>
       </c>
@@ -5351,7 +5354,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>10002169</v>
       </c>
@@ -5377,7 +5380,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>10002170</v>
       </c>
@@ -5403,7 +5406,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>10002171</v>
       </c>
@@ -5429,7 +5432,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>10002172</v>
       </c>
@@ -5455,7 +5458,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>10002173</v>
       </c>
@@ -5481,7 +5484,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>10002174</v>
       </c>
@@ -5507,7 +5510,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>10002175</v>
       </c>
@@ -5533,7 +5536,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>10002176</v>
       </c>
@@ -5559,7 +5562,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>10002177</v>
       </c>
@@ -5585,7 +5588,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>10002178</v>
       </c>
@@ -5611,7 +5614,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>10002179</v>
       </c>
@@ -5637,7 +5640,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>10002180</v>
       </c>

</xml_diff>